<commit_message>
Added demographic data tab to rating scheme
</commit_message>
<xml_diff>
--- a/rating-scheme.xlsx
+++ b/rating-scheme.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\workspace\phd\students\maintainability-tools-comparison\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\workspace\phd\students\microservices-maintainability-benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B859B5BD-F3D3-4217-ABBA-A83E084BC912}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-120" windowWidth="28080" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="-120" windowWidth="28080" windowHeight="16440"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabellenblatt1" sheetId="1" r:id="rId1"/>
+    <sheet name="schema" sheetId="1" r:id="rId1"/>
+    <sheet name="demographics" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>Photo Sharing App</t>
   </si>
@@ -72,16 +72,49 @@
   </si>
   <si>
     <t>Maintainability Rating Scheme</t>
+  </si>
+  <si>
+    <t>Demographic Data</t>
+  </si>
+  <si>
+    <t>Your current role (e.g. software engineer):</t>
+  </si>
+  <si>
+    <t>Years of professional experience:</t>
+  </si>
+  <si>
+    <t>strongly disagree</t>
+  </si>
+  <si>
+    <t>disagree</t>
+  </si>
+  <si>
+    <t>neutral</t>
+  </si>
+  <si>
+    <t>agree</t>
+  </si>
+  <si>
+    <t>strongly agree</t>
+  </si>
+  <si>
+    <t>I am familiar with Microservices.</t>
+  </si>
+  <si>
+    <t>I am familiar with service orientation in general.</t>
+  </si>
+  <si>
+    <t>I am familiar with software quality assurance.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -90,14 +123,17 @@
     <font>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -121,11 +157,18 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="13"/>
       <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -345,11 +388,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -383,19 +427,24 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -706,14 +755,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:H109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -724,10 +773,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="19"/>
     </row>
     <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -753,7 +802,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -776,7 +825,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="10" t="s">
         <v>6</v>
       </c>
@@ -787,7 +836,7 @@
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -810,7 +859,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="10" t="s">
         <v>6</v>
       </c>
@@ -821,7 +870,7 @@
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
@@ -844,7 +893,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="10" t="s">
         <v>6</v>
       </c>
@@ -855,7 +904,7 @@
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -878,7 +927,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="10" t="s">
         <v>6</v>
       </c>
@@ -889,7 +938,7 @@
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="17" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -912,7 +961,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="10" t="s">
         <v>6</v>
       </c>
@@ -923,7 +972,7 @@
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="17" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="9" t="s">
@@ -946,7 +995,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="10" t="s">
         <v>6</v>
       </c>
@@ -957,7 +1006,7 @@
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="17" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="9" t="s">
@@ -980,7 +1029,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="10" t="s">
         <v>6</v>
       </c>
@@ -1067,20 +1116,121 @@
     <mergeCell ref="A11:A12"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Value must be between 1 and 10_x000a_" sqref="C5:G5 C7:G7 C9:G9 C11:G11 C13:G13 C15:G15 C17:G17" xr:uid="{156B71DA-2A4C-44AC-85EC-280C7C88BD08}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Value must be between 1 and 10_x000a_" sqref="C5:G5 C7:G7 C9:G9 C11:G11 C13:G13 C15:G15 C17:G17">
       <formula1>$A$100:$A$109</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A5:A6" r:id="rId1" display="Photo Sharing App" xr:uid="{2DB94A33-0666-4A3E-A068-5FBB7D535C33}"/>
-    <hyperlink ref="A7:A8" r:id="rId2" display="Piggy Metrics" xr:uid="{9CA62D63-FAAC-4AAE-A26A-67A35D75C498}"/>
-    <hyperlink ref="A9:A10" r:id="rId3" display="Robot Shop" xr:uid="{F4E1A95F-11E4-4694-A453-0E339143DBFE}"/>
-    <hyperlink ref="A11:A12" r:id="rId4" display="SB Web Shop v1" xr:uid="{75B5694C-07D2-47EB-91CE-C7BE90246133}"/>
-    <hyperlink ref="A13:A14" r:id="rId5" display="SB Web Shop v2" xr:uid="{8737E5D2-C497-468F-8E5F-7E461D43BB36}"/>
-    <hyperlink ref="A15:A16" r:id="rId6" display="Sock Shop" xr:uid="{524E5914-CE30-4419-915C-D3C60659F984}"/>
-    <hyperlink ref="A17:A18" r:id="rId7" display="Tea Store" xr:uid="{759E3F9D-BE03-4E38-9821-11F1D3B553FB}"/>
+    <hyperlink ref="A5:A6" r:id="rId1" display="Photo Sharing App"/>
+    <hyperlink ref="A7:A8" r:id="rId2" display="Piggy Metrics"/>
+    <hyperlink ref="A9:A10" r:id="rId3" display="Robot Shop"/>
+    <hyperlink ref="A11:A12" r:id="rId4" display="SB Web Shop v1"/>
+    <hyperlink ref="A13:A14" r:id="rId5" display="SB Web Shop v2"/>
+    <hyperlink ref="A15:A16" r:id="rId6" display="Sock Shop"/>
+    <hyperlink ref="A17:A18" r:id="rId7" display="Tea Store"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:B97"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" style="21" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" style="21" customWidth="1"/>
+    <col min="4" max="16384" width="14.42578125" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="20"/>
+    </row>
+    <row r="2" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B9">
+      <formula1>$A$93:$A$97</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>